<commit_message>
Turned output into pandas dataframe
</commit_message>
<xml_diff>
--- a/Wind Renewable Energy/module_data.xlsx
+++ b/Wind Renewable Energy/module_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Home Projects\pvlib-python\Wind Renewable Energy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A576E96-256F-4611-80DD-A10D2B8220CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F934731C-F8DA-4B20-AC07-7845A4A282FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="locations" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>name</t>
   </si>
@@ -71,15 +71,9 @@
     <t>Fresh snow</t>
   </si>
   <si>
-    <t>0.8-0.9</t>
-  </si>
-  <si>
     <t>Sea ice</t>
   </si>
   <si>
-    <t>0.5-0.7</t>
-  </si>
-  <si>
     <t>Desert sand</t>
   </si>
   <si>
@@ -90,9 +84,6 @@
   </si>
   <si>
     <t>Conifer forest</t>
-  </si>
-  <si>
-    <t>0.08-0.15</t>
   </si>
   <si>
     <t>Open ocean</t>
@@ -484,16 +475,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -507,7 +498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -521,7 +512,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -535,7 +526,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -549,85 +540,85 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -643,16 +634,16 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -660,7 +651,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -668,65 +659,65 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="B5" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2">
         <v>0.17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2">
         <v>0.06</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2">
         <v>0.04</v>
@@ -741,11 +732,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B9108C-81EB-404C-9511-FCD1CDF18E9B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed albedo data script and created plot for it
</commit_message>
<xml_diff>
--- a/Wind Renewable Energy/module_data.xlsx
+++ b/Wind Renewable Energy/module_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Home Projects\pvlib-python\Wind Renewable Energy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F37FCC-576D-4EAC-9985-BEC66F38F58A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC41238-2A5D-4DFE-A33B-984EDD841E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22416" yWindow="624" windowWidth="17280" windowHeight="9024" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="locations" sheetId="2" r:id="rId1"/>
@@ -35,9 +35,6 @@
     <t>Substance or Surface</t>
   </si>
   <si>
-    <t> Albedo</t>
-  </si>
-  <si>
     <t>Whole Earth average</t>
   </si>
   <si>
@@ -84,32 +81,22 @@
   </si>
   <si>
     <t>Etc/GMT+7</t>
+  </si>
+  <si>
+    <t>Albedo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9.6"/>
@@ -119,21 +106,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -141,34 +122,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -475,30 +435,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B844AC-15E3-42D6-8BB3-05EE5D385BBA}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -508,11 +468,11 @@
       <c r="C2">
         <v>-134.1739</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -522,11 +482,11 @@
       <c r="C3">
         <v>31.133299999999998</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -536,8 +496,8 @@
       <c r="C4">
         <v>109.34139999999999</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>20</v>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -549,89 +509,89 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAFACE9-3F7B-44A0-A3B9-81CB4442F049}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="1">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="1">
+        <v>0.115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2">
-        <v>0.115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="1">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>0.04</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed issue with location_data and added locations to module_data
</commit_message>
<xml_diff>
--- a/Wind Renewable Energy/module_data.xlsx
+++ b/Wind Renewable Energy/module_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Home Projects\pvlib-python\Wind Renewable Energy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC41238-2A5D-4DFE-A33B-984EDD841E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8800B64-98DF-494E-A39F-1226250C2CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22416" yWindow="624" windowWidth="17280" windowHeight="9024" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="locations" sheetId="2" r:id="rId1"/>
@@ -21,16 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>Juneau, Alaska (USA)</t>
-  </si>
-  <si>
-    <t>Mbabane, Eswatini</t>
-  </si>
-  <si>
-    <t>Pontianak, Indonesia</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Substance or Surface</t>
   </si>
@@ -74,16 +65,67 @@
     <t>timezone</t>
   </si>
   <si>
+    <t>Etc/GMT+2</t>
+  </si>
+  <si>
+    <t>Albedo</t>
+  </si>
+  <si>
+    <t>New York City</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Tokyo</t>
+  </si>
+  <si>
+    <t>Moscow</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro</t>
+  </si>
+  <si>
+    <t>Dubai</t>
+  </si>
+  <si>
+    <t>Cairo</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>Etc/GMT-5</t>
+  </si>
+  <si>
+    <t>Etc/GMT0</t>
+  </si>
+  <si>
+    <t>Etc/GMT+9</t>
+  </si>
+  <si>
+    <t>Etc/GMT+3</t>
+  </si>
+  <si>
+    <t>Etc/GMT+10</t>
+  </si>
+  <si>
+    <t>Etc/GMT+1</t>
+  </si>
+  <si>
+    <t>Etc/GMT-3</t>
+  </si>
+  <si>
+    <t>Etc/GMT+4</t>
+  </si>
+  <si>
     <t>Etc/GMT-8</t>
-  </si>
-  <si>
-    <t>Etc/GMT+2</t>
-  </si>
-  <si>
-    <t>Etc/GMT+7</t>
-  </si>
-  <si>
-    <t>Albedo</t>
   </si>
 </sst>
 </file>
@@ -126,10 +168,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -433,71 +478,172 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B844AC-15E3-42D6-8BB3-05EE5D385BBA}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2">
+        <v>40.712800000000001</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-74.006</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2">
+        <v>51.507399999999997</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-0.1278</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2">
+        <v>35.689500000000002</v>
+      </c>
+      <c r="C4" s="2">
+        <v>139.6917</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2">
+        <v>55.755800000000001</v>
+      </c>
+      <c r="C5" s="2">
+        <v>37.6173</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2">
+        <v>-33.8688</v>
+      </c>
+      <c r="C6" s="2">
+        <v>151.20930000000001</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2">
+        <v>48.8566</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2.3521999999999998</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-22.9068</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-43.172899999999998</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2">
+        <v>25.204799999999999</v>
+      </c>
+      <c r="C9" s="2">
+        <v>55.270800000000001</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2">
+        <v>30.0444</v>
+      </c>
+      <c r="C10" s="2">
+        <v>31.235700000000001</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>58.454599999999999</v>
-      </c>
-      <c r="C2">
-        <v>-134.1739</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>-26.316700000000001</v>
-      </c>
-      <c r="C3">
-        <v>31.133299999999998</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>-2.06E-2</v>
-      </c>
-      <c r="C4">
-        <v>109.34139999999999</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2">
+        <v>34.052199999999999</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-118.2437</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -509,7 +655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAFACE9-3F7B-44A0-A3B9-81CB4442F049}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -517,15 +663,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>0.3</v>
@@ -533,7 +679,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>0.85</v>
@@ -541,7 +687,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>0.6</v>
@@ -549,7 +695,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>0.4</v>
@@ -557,7 +703,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>0.25</v>
@@ -565,7 +711,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>0.17</v>
@@ -573,7 +719,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>0.115</v>
@@ -581,7 +727,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>0.06</v>
@@ -589,7 +735,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>0.04</v>

</xml_diff>

<commit_message>
Fixed issue with x ticks overlapping, added output to excel file
</commit_message>
<xml_diff>
--- a/Wind Renewable Energy/module_data.xlsx
+++ b/Wind Renewable Energy/module_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Home Projects\pvlib-python\Wind Renewable Energy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8800B64-98DF-494E-A39F-1226250C2CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1026F030-0A1B-4690-B606-0B1757E37A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="locations" sheetId="2" r:id="rId1"/>
@@ -480,19 +480,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B844AC-15E3-42D6-8BB3-05EE5D385BBA}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -506,7 +506,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -520,7 +520,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -534,7 +534,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -548,7 +548,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -562,7 +562,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -576,7 +576,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -590,7 +590,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -604,7 +604,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -618,7 +618,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -632,7 +632,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -655,13 +655,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAFACE9-3F7B-44A0-A3B9-81CB4442F049}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,39 +669,39 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -709,39 +709,42 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
-        <v>0.115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B10" s="1">
-        <v>0.04</v>
+        <v>0.85</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B10">
+    <sortCondition ref="B1:B10"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final changes to code
</commit_message>
<xml_diff>
--- a/Wind Renewable Energy/module_data.xlsx
+++ b/Wind Renewable Energy/module_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Home Projects\pvlib-python\Wind Renewable Energy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1026F030-0A1B-4690-B606-0B1757E37A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898CA0FA-7A31-47EF-971D-9875840A57CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="locations" sheetId="2" r:id="rId1"/>
@@ -180,7 +180,99 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -191,6 +283,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{99516E62-EEEF-462D-9EBF-FA46144161AE}" name="Table1" displayName="Table1" ref="A1:D11" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="A1:D11" xr:uid="{99516E62-EEEF-462D-9EBF-FA46144161AE}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{43A6F3A6-6EC1-401C-BCF8-86C4F54EC170}" name="name" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{5A7FACC9-AB9C-4217-BE34-7B1936DE765F}" name="latitude" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{3C4C6BC5-8F41-4CE5-8B21-C4D79225A739}" name="longitude" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{343F5988-0FCA-485A-BB18-12CDEC10FAD6}" name="timezone" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A56243BD-7076-4654-AE05-1E0E8E0AB199}" name="Table2" displayName="Table2" ref="A1:B10" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:B10" xr:uid="{A56243BD-7076-4654-AE05-1E0E8E0AB199}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{9BF92B50-F089-4B44-B52C-08581DEC1934}" name="Substance or Surface" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{85C50132-EF08-4653-9826-60F8EF12D716}" name="Albedo" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -481,14 +597,14 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.88671875" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -648,6 +764,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -656,10 +775,14 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -746,5 +869,8 @@
     <sortCondition ref="B1:B10"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed issue with albedos graph and change locations output to be in order of latitude
</commit_message>
<xml_diff>
--- a/Wind Renewable Energy/module_data.xlsx
+++ b/Wind Renewable Energy/module_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Home Projects\pvlib-python\Wind Renewable Energy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898CA0FA-7A31-47EF-971D-9875840A57CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47FAB65-1AF6-4146-8A93-C768218D7E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="locations" sheetId="2" r:id="rId1"/>
@@ -286,24 +286,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{99516E62-EEEF-462D-9EBF-FA46144161AE}" name="Table1" displayName="Table1" ref="A1:D11" totalsRowShown="0" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{99516E62-EEEF-462D-9EBF-FA46144161AE}" name="Table1" displayName="Table1" ref="A1:D11" totalsRowShown="0" dataDxfId="8">
   <autoFilter ref="A1:D11" xr:uid="{99516E62-EEEF-462D-9EBF-FA46144161AE}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D11">
+    <sortCondition ref="C1:C11"/>
+  </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{43A6F3A6-6EC1-401C-BCF8-86C4F54EC170}" name="name" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{5A7FACC9-AB9C-4217-BE34-7B1936DE765F}" name="latitude" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{3C4C6BC5-8F41-4CE5-8B21-C4D79225A739}" name="longitude" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{343F5988-0FCA-485A-BB18-12CDEC10FAD6}" name="timezone" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{43A6F3A6-6EC1-401C-BCF8-86C4F54EC170}" name="name" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{5A7FACC9-AB9C-4217-BE34-7B1936DE765F}" name="latitude" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{3C4C6BC5-8F41-4CE5-8B21-C4D79225A739}" name="longitude" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{343F5988-0FCA-485A-BB18-12CDEC10FAD6}" name="timezone" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A56243BD-7076-4654-AE05-1E0E8E0AB199}" name="Table2" displayName="Table2" ref="A1:B10" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A56243BD-7076-4654-AE05-1E0E8E0AB199}" name="Table2" displayName="Table2" ref="A1:B10" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:B10" xr:uid="{A56243BD-7076-4654-AE05-1E0E8E0AB199}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{9BF92B50-F089-4B44-B52C-08581DEC1934}" name="Substance or Surface" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{85C50132-EF08-4653-9826-60F8EF12D716}" name="Albedo" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{9BF92B50-F089-4B44-B52C-08581DEC1934}" name="Substance or Surface" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{85C50132-EF08-4653-9826-60F8EF12D716}" name="Albedo" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -596,19 +599,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B844AC-15E3-42D6-8BB3-05EE5D385BBA}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -622,105 +625,105 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2">
+        <v>34.052199999999999</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-118.2437</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B3" s="2">
         <v>40.712800000000001</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C3" s="2">
         <v>-74.006</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-22.9068</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-43.172899999999998</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B5" s="2">
         <v>51.507399999999997</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C5" s="2">
         <v>-0.1278</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2">
-        <v>35.689500000000002</v>
-      </c>
-      <c r="C4" s="2">
-        <v>139.6917</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2">
+        <v>48.8566</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2.3521999999999998</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2">
+        <v>30.0444</v>
+      </c>
+      <c r="C7" s="2">
+        <v>31.235700000000001</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B8" s="2">
         <v>55.755800000000001</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C8" s="2">
         <v>37.6173</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="2">
-        <v>-33.8688</v>
-      </c>
-      <c r="C6" s="2">
-        <v>151.20930000000001</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="2">
-        <v>48.8566</v>
-      </c>
-      <c r="C7" s="2">
-        <v>2.3521999999999998</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="2">
-        <v>-22.9068</v>
-      </c>
-      <c r="C8" s="2">
-        <v>-43.172899999999998</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -734,32 +737,32 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2">
-        <v>30.0444</v>
+        <v>35.689500000000002</v>
       </c>
       <c r="C10" s="2">
-        <v>31.235700000000001</v>
+        <v>139.6917</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2">
-        <v>34.052199999999999</v>
+        <v>-33.8688</v>
       </c>
       <c r="C11" s="2">
-        <v>-118.2437</v>
+        <v>151.20930000000001</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -774,17 +777,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAFACE9-3F7B-44A0-A3B9-81CB4442F049}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -792,7 +795,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -800,7 +803,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -808,7 +811,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -816,7 +819,7 @@
         <v>0.115</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -824,7 +827,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -832,7 +835,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -840,7 +843,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -848,7 +851,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -856,7 +859,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>